<commit_message>
fixed harvester column in rnasamples -- holly changed some of the bioSample names to H.BROWN
</commit_message>
<xml_diff>
--- a/old_database/crypto/rnaSample/rnaSample_1874.xlsx
+++ b/old_database/crypto/rnaSample/rnaSample_1874.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">10.25.16</t>
   </si>
   <si>
-    <t xml:space="preserve">S.GISH</t>
+    <t xml:space="preserve">H.BROWN</t>
   </si>
   <si>
     <t xml:space="preserve">Retrofitted_1874</t>
@@ -181,7 +181,7 @@
   </sheetPr>
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>

</xml_diff>